<commit_message>
imagesv for 60, 45
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>Jackie's 4920 Hours - Baker/ Nicole research</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>Week 12</t>
+  </si>
+  <si>
+    <t>Week 13</t>
   </si>
 </sst>
 </file>
@@ -521,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I72"/>
+  <dimension ref="B2:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -546,7 +549,7 @@
       </c>
       <c r="C4" s="4">
         <f>SUM(E:E)</f>
-        <v>61.399999999999977</v>
+        <v>68.483333333333306</v>
       </c>
       <c r="E4" s="4"/>
     </row>
@@ -645,7 +648,7 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="E10" s="4">
-        <f t="shared" ref="E10:E72" si="0">(D10-C10)*24</f>
+        <f t="shared" ref="E10:E74" si="0">(D10-C10)*24</f>
         <v>0.50000000000000089</v>
       </c>
       <c r="G10" s="3" t="s">
@@ -803,8 +806,8 @@
         <v>27</v>
       </c>
       <c r="H17" s="4">
-        <f>SUM(E62:E75)</f>
-        <v>8.7500000000000036</v>
+        <f>SUM(E62:E72)</f>
+        <v>9.3333333333333357</v>
       </c>
     </row>
     <row r="18" spans="2:8">
@@ -821,6 +824,13 @@
         <f t="shared" si="0"/>
         <v>1.9166666666666652</v>
       </c>
+      <c r="G18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H18" s="4">
+        <f>SUM(E73:E79)</f>
+        <v>6.4999999999999982</v>
+      </c>
     </row>
     <row r="19" spans="2:8">
       <c r="C19" s="2">
@@ -1581,6 +1591,39 @@
         <v>0.58333333333333126</v>
       </c>
       <c r="F72" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6">
+      <c r="B73" s="5">
+        <v>42856</v>
+      </c>
+      <c r="C73" s="2">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="D73" s="2">
+        <v>0.67013888888888884</v>
+      </c>
+      <c r="E73" s="4">
+        <f t="shared" si="0"/>
+        <v>4.2499999999999982</v>
+      </c>
+      <c r="F73" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6">
+      <c r="C74" s="2">
+        <v>0.73263888888888884</v>
+      </c>
+      <c r="D74" s="2">
+        <v>0.82638888888888884</v>
+      </c>
+      <c r="E74" s="4">
+        <f t="shared" si="0"/>
+        <v>2.25</v>
+      </c>
+      <c r="F74" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding displays for presentation
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -524,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I74"/>
+  <dimension ref="B2:I75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -549,7 +549,7 @@
       </c>
       <c r="C4" s="4">
         <f>SUM(E:E)</f>
-        <v>68.483333333333306</v>
+        <v>69.316666666666634</v>
       </c>
       <c r="E4" s="4"/>
     </row>
@@ -648,7 +648,7 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="E10" s="4">
-        <f t="shared" ref="E10:E74" si="0">(D10-C10)*24</f>
+        <f t="shared" ref="E10:E75" si="0">(D10-C10)*24</f>
         <v>0.50000000000000089</v>
       </c>
       <c r="G10" s="3" t="s">
@@ -829,7 +829,7 @@
       </c>
       <c r="H18" s="4">
         <f>SUM(E73:E79)</f>
-        <v>6.4999999999999982</v>
+        <v>7.3333333333333313</v>
       </c>
     </row>
     <row r="19" spans="2:8">
@@ -1625,6 +1625,21 @@
       </c>
       <c r="F74" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6">
+      <c r="B75" s="5">
+        <v>42857</v>
+      </c>
+      <c r="C75" s="2">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="D75" s="2">
+        <v>0.53819444444444442</v>
+      </c>
+      <c r="E75" s="4">
+        <f t="shared" si="0"/>
+        <v>0.83333333333333304</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started doing it in MATLAB
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -379,11 +379,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2139446616"/>
-        <c:axId val="2139449640"/>
+        <c:axId val="2074855704"/>
+        <c:axId val="2074858824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2139446616"/>
+        <c:axId val="2074855704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -392,12 +392,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2139449640"/>
+        <c:crossAx val="2074858824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2139449640"/>
+        <c:axId val="2074858824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -408,7 +408,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2139446616"/>
+        <c:crossAx val="2074855704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -502,7 +502,7 @@
                   <c:v>25.33333333333334</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.66666666666666</c:v>
+                  <c:v>24.08333333333332</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -517,11 +517,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2139485720"/>
-        <c:axId val="2139488680"/>
+        <c:axId val="2046740120"/>
+        <c:axId val="2046743144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2139485720"/>
+        <c:axId val="2046740120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -530,12 +530,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2139488680"/>
+        <c:crossAx val="2046743144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2139488680"/>
+        <c:axId val="2046743144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -547,7 +547,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2139485720"/>
+        <c:crossAx val="2046740120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2572,10 +2572,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J110"/>
+  <dimension ref="B2:J111"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+      <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="C4" s="4">
         <f>SUM(E:E)</f>
-        <v>129.00000000000006</v>
+        <v>138.41666666666674</v>
       </c>
     </row>
     <row r="5" spans="2:10">
@@ -2606,7 +2606,7 @@
       </c>
       <c r="C5" s="4">
         <f>AVERAGE(I7:I21)</f>
-        <v>25.8</v>
+        <v>27.68333333333333</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -2662,7 +2662,7 @@
         <v>0.62152777777777779</v>
       </c>
       <c r="E9" s="4">
-        <f t="shared" ref="E9:E83" si="0">(D9-C9)*24</f>
+        <f t="shared" ref="E9:E87" si="0">(D9-C9)*24</f>
         <v>2.4166666666666661</v>
       </c>
       <c r="H9" s="3" t="s">
@@ -2720,8 +2720,8 @@
         <v>14</v>
       </c>
       <c r="I11" s="4">
-        <f>SUM(E76:E88)</f>
-        <v>14.666666666666664</v>
+        <f>SUM(E76:E89)</f>
+        <v>24.083333333333321</v>
       </c>
     </row>
     <row r="12" spans="2:10">
@@ -3475,7 +3475,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="65" spans="2:6">
+    <row r="65" spans="2:7">
       <c r="C65" s="2">
         <v>0.71180555555555547</v>
       </c>
@@ -3490,7 +3490,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="66" spans="2:6">
+    <row r="66" spans="2:7">
       <c r="C66" s="2">
         <v>0.78819444444444453</v>
       </c>
@@ -3502,7 +3502,7 @@
         <v>0.6666666666666643</v>
       </c>
     </row>
-    <row r="67" spans="2:6">
+    <row r="67" spans="2:7">
       <c r="B67" s="5">
         <v>42921</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>2.6666666666666652</v>
       </c>
     </row>
-    <row r="68" spans="2:6">
+    <row r="68" spans="2:7">
       <c r="C68" s="2">
         <v>0.65277777777777779</v>
       </c>
@@ -3529,7 +3529,7 @@
         <v>3.1666666666666661</v>
       </c>
     </row>
-    <row r="69" spans="2:6">
+    <row r="69" spans="2:7">
       <c r="B69" s="5"/>
       <c r="C69" s="2">
         <v>0.875</v>
@@ -3542,7 +3542,7 @@
         <v>1.9166666666666679</v>
       </c>
     </row>
-    <row r="70" spans="2:6">
+    <row r="70" spans="2:7">
       <c r="B70" s="5">
         <v>42922</v>
       </c>
@@ -3560,7 +3560,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="71" spans="2:6">
+    <row r="71" spans="2:7">
       <c r="C71" s="2">
         <v>0.4375</v>
       </c>
@@ -3572,7 +3572,7 @@
         <v>1.6666666666666661</v>
       </c>
     </row>
-    <row r="72" spans="2:6">
+    <row r="72" spans="2:7">
       <c r="C72" s="2">
         <v>0.51736111111111105</v>
       </c>
@@ -3584,7 +3584,7 @@
         <v>3.7500000000000027</v>
       </c>
     </row>
-    <row r="73" spans="2:6">
+    <row r="73" spans="2:7">
       <c r="B73" s="5">
         <v>42923</v>
       </c>
@@ -3599,7 +3599,7 @@
         <v>2.1666666666666656</v>
       </c>
     </row>
-    <row r="74" spans="2:6">
+    <row r="74" spans="2:7">
       <c r="B74" s="5"/>
       <c r="C74" s="2">
         <v>0.50694444444444442</v>
@@ -3612,7 +3612,7 @@
         <v>1.3333333333333339</v>
       </c>
     </row>
-    <row r="75" spans="2:6">
+    <row r="75" spans="2:7">
       <c r="B75" s="5">
         <v>42925</v>
       </c>
@@ -3627,7 +3627,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="76" spans="2:6">
+    <row r="76" spans="2:7">
       <c r="B76" s="5">
         <v>42926</v>
       </c>
@@ -3642,7 +3642,7 @@
         <v>0.33333333333333215</v>
       </c>
     </row>
-    <row r="77" spans="2:6">
+    <row r="77" spans="2:7">
       <c r="B77" s="5"/>
       <c r="C77" s="2">
         <v>0.37152777777777773</v>
@@ -3654,8 +3654,9 @@
         <f t="shared" si="0"/>
         <v>4.3333333333333357</v>
       </c>
-    </row>
-    <row r="78" spans="2:6">
+      <c r="G77" s="4"/>
+    </row>
+    <row r="78" spans="2:7">
       <c r="C78" s="2">
         <v>0.58333333333333337</v>
       </c>
@@ -3666,8 +3667,9 @@
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-    </row>
-    <row r="79" spans="2:6">
+      <c r="G78" s="4"/>
+    </row>
+    <row r="79" spans="2:7">
       <c r="C79" s="2">
         <v>0.83333333333333337</v>
       </c>
@@ -3678,8 +3680,9 @@
         <f t="shared" si="0"/>
         <v>0.33333333333333215</v>
       </c>
-    </row>
-    <row r="80" spans="2:6">
+      <c r="G79" s="4"/>
+    </row>
+    <row r="80" spans="2:7">
       <c r="B80" s="5">
         <v>42927</v>
       </c>
@@ -3694,7 +3697,7 @@
         <v>1.416666666666667</v>
       </c>
     </row>
-    <row r="81" spans="2:5">
+    <row r="81" spans="2:7">
       <c r="C81" s="2">
         <v>0.64930555555555558</v>
       </c>
@@ -3706,7 +3709,7 @@
         <v>3.4999999999999982</v>
       </c>
     </row>
-    <row r="82" spans="2:5">
+    <row r="82" spans="2:7">
       <c r="B82" s="5">
         <v>42928</v>
       </c>
@@ -3714,91 +3717,127 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="D82" s="2">
-        <v>0.5</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="E82" s="4">
         <f t="shared" si="0"/>
-        <v>1.9999999999999996</v>
-      </c>
-    </row>
-    <row r="83" spans="2:5">
+        <v>3.7499999999999987</v>
+      </c>
+      <c r="G82" s="4"/>
+    </row>
+    <row r="83" spans="2:7">
       <c r="C83" s="2">
-        <v>0.54166666666666663</v>
+        <v>0.59375</v>
       </c>
       <c r="D83" s="2">
-        <v>0.625</v>
+        <v>0.63541666666666663</v>
       </c>
       <c r="E83" s="4">
         <f t="shared" si="0"/>
-        <v>2.0000000000000009</v>
-      </c>
-    </row>
-    <row r="84" spans="2:5">
-      <c r="C84" s="2"/>
-      <c r="D84" s="2"/>
-      <c r="E84" s="4"/>
-    </row>
-    <row r="85" spans="2:5">
-      <c r="C85" s="2"/>
-      <c r="D85" s="2"/>
-      <c r="E85" s="4"/>
-    </row>
-    <row r="86" spans="2:5">
+        <v>0.99999999999999911</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7">
+      <c r="B84" s="5">
+        <v>42929</v>
+      </c>
+      <c r="C84" s="2">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="D84" s="2">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="E84" s="4">
+        <f t="shared" si="0"/>
+        <v>0.49999999999999822</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7">
+      <c r="B85" s="5">
+        <v>42930</v>
+      </c>
+      <c r="C85" s="2">
+        <v>0.37847222222222227</v>
+      </c>
+      <c r="D85" s="2">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="E85" s="4">
+        <f t="shared" si="0"/>
+        <v>0.58333333333333126</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7">
       <c r="B86" s="5"/>
-      <c r="C86" s="2"/>
-      <c r="D86" s="2"/>
-      <c r="E86" s="4"/>
-    </row>
-    <row r="87" spans="2:5">
+      <c r="C86" s="2">
+        <v>0.4201388888888889</v>
+      </c>
+      <c r="D86" s="2">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="E86" s="4">
+        <f t="shared" si="0"/>
+        <v>1.583333333333333</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7">
       <c r="B87" s="5"/>
-      <c r="C87" s="2"/>
-      <c r="D87" s="2"/>
-      <c r="E87" s="4"/>
-    </row>
-    <row r="88" spans="2:5">
+      <c r="C87" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="D87" s="2">
+        <v>0.8125</v>
+      </c>
+      <c r="E87" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7">
+      <c r="B88" s="5"/>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
       <c r="E88" s="4"/>
     </row>
-    <row r="89" spans="2:5">
-      <c r="B89" s="5"/>
+    <row r="89" spans="2:7">
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
       <c r="E89" s="4"/>
     </row>
-    <row r="90" spans="2:5">
+    <row r="90" spans="2:7">
+      <c r="B90" s="5"/>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
       <c r="E90" s="4"/>
     </row>
-    <row r="91" spans="2:5">
+    <row r="91" spans="2:7">
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
       <c r="E91" s="4"/>
     </row>
-    <row r="92" spans="2:5">
+    <row r="92" spans="2:7">
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
       <c r="E92" s="4"/>
     </row>
-    <row r="93" spans="2:5">
-      <c r="B93" s="5"/>
+    <row r="93" spans="2:7">
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
       <c r="E93" s="4"/>
     </row>
-    <row r="94" spans="2:5">
+    <row r="94" spans="2:7">
+      <c r="B94" s="5"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
       <c r="E94" s="4"/>
     </row>
-    <row r="95" spans="2:5">
-      <c r="B95" s="5"/>
+    <row r="95" spans="2:7">
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
       <c r="E95" s="4"/>
     </row>
-    <row r="96" spans="2:5">
+    <row r="96" spans="2:7">
+      <c r="B96" s="5"/>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
       <c r="E96" s="4"/>
@@ -3819,18 +3858,17 @@
       <c r="E99" s="4"/>
     </row>
     <row r="100" spans="2:5">
-      <c r="B100" s="5"/>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
       <c r="E100" s="4"/>
     </row>
     <row r="101" spans="2:5">
+      <c r="B101" s="5"/>
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
       <c r="E101" s="4"/>
     </row>
     <row r="102" spans="2:5">
-      <c r="B102" s="5"/>
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
       <c r="E102" s="4"/>
@@ -3848,6 +3886,7 @@
       <c r="E104" s="4"/>
     </row>
     <row r="105" spans="2:5">
+      <c r="B105" s="5"/>
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
       <c r="E105" s="4"/>
@@ -3873,10 +3912,15 @@
       <c r="E109" s="4"/>
     </row>
     <row r="110" spans="2:5">
-      <c r="B110" s="5"/>
       <c r="C110" s="2"/>
       <c r="D110" s="2"/>
       <c r="E110" s="4"/>
+    </row>
+    <row r="111" spans="2:5">
+      <c r="B111" s="5"/>
+      <c r="C111" s="2"/>
+      <c r="D111" s="2"/>
+      <c r="E111" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
making it work in MATLAB
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -379,11 +379,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2074855704"/>
-        <c:axId val="2074858824"/>
+        <c:axId val="2126520168"/>
+        <c:axId val="2126517096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2074855704"/>
+        <c:axId val="2126520168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -392,12 +392,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2074858824"/>
+        <c:crossAx val="2126517096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2074858824"/>
+        <c:axId val="2126517096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -408,7 +408,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2074855704"/>
+        <c:crossAx val="2126520168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -502,7 +502,7 @@
                   <c:v>25.33333333333334</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24.91666666666666</c:v>
+                  <c:v>28.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -517,11 +517,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2046740120"/>
-        <c:axId val="2046743144"/>
+        <c:axId val="2127605784"/>
+        <c:axId val="2127602760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2046740120"/>
+        <c:axId val="2127605784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -530,12 +530,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2046743144"/>
+        <c:crossAx val="2127602760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2046743144"/>
+        <c:axId val="2127602760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -547,7 +547,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2046740120"/>
+        <c:crossAx val="2127605784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2574,8 +2574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E88" sqref="E88"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="C4" s="4">
         <f>SUM(E:E)</f>
-        <v>139.25000000000006</v>
+        <v>142.5833333333334</v>
       </c>
     </row>
     <row r="5" spans="2:10">
@@ -2606,7 +2606,7 @@
       </c>
       <c r="C5" s="4">
         <f>AVERAGE(I7:I21)</f>
-        <v>27.85</v>
+        <v>28.516666666666669</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -2662,7 +2662,7 @@
         <v>0.62152777777777779</v>
       </c>
       <c r="E9" s="4">
-        <f t="shared" ref="E9:E88" si="0">(D9-C9)*24</f>
+        <f t="shared" ref="E9:E91" si="0">(D9-C9)*24</f>
         <v>2.4166666666666661</v>
       </c>
       <c r="H9" s="3" t="s">
@@ -2721,7 +2721,7 @@
       </c>
       <c r="I11" s="4">
         <f>SUM(E76:E95)</f>
-        <v>24.916666666666661</v>
+        <v>28.249999999999996</v>
       </c>
     </row>
     <row r="12" spans="2:10">
@@ -3804,23 +3804,47 @@
         <f t="shared" si="0"/>
         <v>6.666666666666667</v>
       </c>
+      <c r="G88" s="4"/>
     </row>
     <row r="89" spans="2:7">
-      <c r="B89" s="5"/>
-      <c r="C89" s="2"/>
-      <c r="D89" s="2"/>
-      <c r="E89" s="4"/>
+      <c r="B89" s="5">
+        <v>42932</v>
+      </c>
+      <c r="C89" s="2">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="D89" s="2">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="E89" s="4">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
     </row>
     <row r="90" spans="2:7">
-      <c r="C90" s="2"/>
-      <c r="D90" s="2"/>
-      <c r="E90" s="4"/>
+      <c r="C90" s="2">
+        <v>0.70138888888888884</v>
+      </c>
+      <c r="D90" s="2">
+        <v>0.74652777777777779</v>
+      </c>
+      <c r="E90" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0833333333333348</v>
+      </c>
     </row>
     <row r="91" spans="2:7">
       <c r="B91" s="5"/>
-      <c r="C91" s="2"/>
-      <c r="D91" s="2"/>
-      <c r="E91" s="4"/>
+      <c r="C91" s="2">
+        <v>0.75347222222222221</v>
+      </c>
+      <c r="D91" s="2">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="E91" s="4">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
     </row>
     <row r="92" spans="2:7">
       <c r="C92" s="2"/>

</xml_diff>

<commit_message>
got indent defined in MATLAB
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -379,11 +379,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2126520168"/>
-        <c:axId val="2126517096"/>
+        <c:axId val="2083176376"/>
+        <c:axId val="2083957944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2126520168"/>
+        <c:axId val="2083176376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -392,12 +392,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126517096"/>
+        <c:crossAx val="2083957944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2126517096"/>
+        <c:axId val="2083957944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -408,7 +408,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126520168"/>
+        <c:crossAx val="2083176376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -504,6 +504,9 @@
                 <c:pt idx="4">
                   <c:v>28.33333333333333</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.083333333333332</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -517,11 +520,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2127605784"/>
-        <c:axId val="2127602760"/>
+        <c:axId val="2083991128"/>
+        <c:axId val="2083994152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2127605784"/>
+        <c:axId val="2083991128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -530,12 +533,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127602760"/>
+        <c:crossAx val="2083994152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2127602760"/>
+        <c:axId val="2083994152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -547,7 +550,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127605784"/>
+        <c:crossAx val="2083991128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2574,8 +2577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E91" sqref="E91"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2597,7 +2600,7 @@
       </c>
       <c r="C4" s="4">
         <f>SUM(E:E)</f>
-        <v>142.66666666666671</v>
+        <v>148.75000000000003</v>
       </c>
     </row>
     <row r="5" spans="2:10">
@@ -2606,7 +2609,7 @@
       </c>
       <c r="C5" s="4">
         <f>AVERAGE(I7:I21)</f>
-        <v>28.533333333333339</v>
+        <v>24.791666666666671</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -2662,7 +2665,7 @@
         <v>0.62152777777777779</v>
       </c>
       <c r="E9" s="4">
-        <f t="shared" ref="E9:E91" si="0">(D9-C9)*24</f>
+        <f t="shared" ref="E9:E94" si="0">(D9-C9)*24</f>
         <v>2.4166666666666661</v>
       </c>
       <c r="H9" s="3" t="s">
@@ -2720,7 +2723,7 @@
         <v>14</v>
       </c>
       <c r="I11" s="4">
-        <f>SUM(E76:E95)</f>
+        <f>SUM(E76:E91)</f>
         <v>28.333333333333329</v>
       </c>
     </row>
@@ -2739,7 +2742,10 @@
       <c r="H12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="4"/>
+      <c r="I12" s="4">
+        <f>SUM(E92:E106)</f>
+        <v>6.0833333333333321</v>
+      </c>
     </row>
     <row r="13" spans="2:10">
       <c r="B13" s="5"/>
@@ -3847,19 +3853,43 @@
       </c>
     </row>
     <row r="92" spans="2:7">
-      <c r="C92" s="2"/>
-      <c r="D92" s="2"/>
-      <c r="E92" s="4"/>
+      <c r="B92" s="5">
+        <v>42933</v>
+      </c>
+      <c r="C92" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="D92" s="2">
+        <v>0.49652777777777773</v>
+      </c>
+      <c r="E92" s="4">
+        <f t="shared" si="0"/>
+        <v>2.9166666666666656</v>
+      </c>
     </row>
     <row r="93" spans="2:7">
-      <c r="C93" s="2"/>
-      <c r="D93" s="2"/>
-      <c r="E93" s="4"/>
+      <c r="C93" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D93" s="2">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="E93" s="4">
+        <f t="shared" si="0"/>
+        <v>1.1666666666666679</v>
+      </c>
     </row>
     <row r="94" spans="2:7">
-      <c r="C94" s="2"/>
-      <c r="D94" s="2"/>
-      <c r="E94" s="4"/>
+      <c r="C94" s="2">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="D94" s="2">
+        <v>0.80555555555555547</v>
+      </c>
+      <c r="E94" s="4">
+        <f t="shared" si="0"/>
+        <v>1.9999999999999982</v>
+      </c>
     </row>
     <row r="95" spans="2:7">
       <c r="B95" s="5"/>

</xml_diff>

<commit_message>
matlab code to detect AFM area
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -379,11 +379,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2083176376"/>
-        <c:axId val="2083957944"/>
+        <c:axId val="2067173576"/>
+        <c:axId val="2081622440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2083176376"/>
+        <c:axId val="2067173576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -392,12 +392,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2083957944"/>
+        <c:crossAx val="2081622440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2083957944"/>
+        <c:axId val="2081622440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -408,7 +408,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2083176376"/>
+        <c:crossAx val="2067173576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -505,7 +505,7 @@
                   <c:v>28.33333333333333</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.833333333333332</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -520,11 +520,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2083991128"/>
-        <c:axId val="2083994152"/>
+        <c:axId val="2083037880"/>
+        <c:axId val="2083078168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2083991128"/>
+        <c:axId val="2083037880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -533,12 +533,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2083994152"/>
+        <c:crossAx val="2083078168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2083994152"/>
+        <c:axId val="2083078168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -550,7 +550,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2083991128"/>
+        <c:crossAx val="2083037880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2577,8 +2577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D95" sqref="D95"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2600,7 +2600,7 @@
       </c>
       <c r="C4" s="4">
         <f>SUM(E:E)</f>
-        <v>148.50000000000003</v>
+        <v>154.16666666666671</v>
       </c>
     </row>
     <row r="5" spans="2:10">
@@ -2609,7 +2609,7 @@
       </c>
       <c r="C5" s="4">
         <f>AVERAGE(I7:I21)</f>
-        <v>24.750000000000004</v>
+        <v>25.694444444444446</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -2665,7 +2665,7 @@
         <v>0.62152777777777779</v>
       </c>
       <c r="E9" s="4">
-        <f t="shared" ref="E9:E94" si="0">(D9-C9)*24</f>
+        <f t="shared" ref="E9:E96" si="0">(D9-C9)*24</f>
         <v>2.4166666666666661</v>
       </c>
       <c r="H9" s="3" t="s">
@@ -2744,7 +2744,7 @@
       </c>
       <c r="I12" s="4">
         <f>SUM(E92:E106)</f>
-        <v>5.833333333333333</v>
+        <v>11.499999999999998</v>
       </c>
     </row>
     <row r="13" spans="2:10">
@@ -3892,15 +3892,31 @@
       </c>
     </row>
     <row r="95" spans="2:7">
-      <c r="B95" s="5"/>
-      <c r="C95" s="2"/>
-      <c r="D95" s="2"/>
-      <c r="E95" s="4"/>
+      <c r="B95" s="5">
+        <v>42934</v>
+      </c>
+      <c r="C95" s="2">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="D95" s="2">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="E95" s="4">
+        <f t="shared" si="0"/>
+        <v>8.3333333333331705E-2</v>
+      </c>
     </row>
     <row r="96" spans="2:7">
-      <c r="C96" s="2"/>
-      <c r="D96" s="2"/>
-      <c r="E96" s="4"/>
+      <c r="C96" s="2">
+        <v>0.4548611111111111</v>
+      </c>
+      <c r="D96" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="E96" s="4">
+        <f t="shared" si="0"/>
+        <v>5.5833333333333339</v>
+      </c>
     </row>
     <row r="97" spans="2:5">
       <c r="B97" s="5"/>

</xml_diff>

<commit_message>
afm data, notes + hours
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="0" windowWidth="25600" windowHeight="13240" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="13240" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="hours" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>Day off</t>
+  </si>
+  <si>
+    <t>Sick</t>
   </si>
 </sst>
 </file>
@@ -379,11 +382,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2067173576"/>
-        <c:axId val="2081622440"/>
+        <c:axId val="2103524248"/>
+        <c:axId val="2103521176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2067173576"/>
+        <c:axId val="2103524248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -392,12 +395,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081622440"/>
+        <c:crossAx val="2103521176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2081622440"/>
+        <c:axId val="2103521176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -408,7 +411,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2067173576"/>
+        <c:crossAx val="2103524248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -455,7 +458,7 @@
             <c:strRef>
               <c:f>summer!$H$7:$H$21</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Week 1</c:v>
                 </c:pt>
@@ -479,6 +482,12 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Week 8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Week 9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Week 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -505,7 +514,10 @@
                   <c:v>28.33333333333333</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.333333333333332</c:v>
+                  <c:v>16.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -520,11 +532,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2083037880"/>
-        <c:axId val="2083078168"/>
+        <c:axId val="2097188776"/>
+        <c:axId val="2097191800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2083037880"/>
+        <c:axId val="2097188776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -533,12 +545,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2083078168"/>
+        <c:crossAx val="2097191800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2083078168"/>
+        <c:axId val="2097191800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -550,7 +562,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2083037880"/>
+        <c:crossAx val="2097188776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2575,10 +2587,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J110"/>
+  <dimension ref="B2:J116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D98" sqref="D98"/>
+    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E116" sqref="E116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2600,7 +2612,11 @@
       </c>
       <c r="C4" s="4">
         <f>SUM(E:E)</f>
-        <v>151.00000000000006</v>
+        <v>171.83333333333346</v>
+      </c>
+      <c r="F4">
+        <f>3*4*16</f>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="2:10">
@@ -2609,7 +2625,7 @@
       </c>
       <c r="C5" s="4">
         <f>AVERAGE(I7:I21)</f>
-        <v>25.166666666666671</v>
+        <v>24.547619047619047</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -2665,7 +2681,7 @@
         <v>0.62152777777777779</v>
       </c>
       <c r="E9" s="4">
-        <f t="shared" ref="E9:E97" si="0">(D9-C9)*24</f>
+        <f t="shared" ref="E9:E116" si="0">(D9-C9)*24</f>
         <v>2.4166666666666661</v>
       </c>
       <c r="H9" s="3" t="s">
@@ -2726,6 +2742,9 @@
         <f>SUM(E76:E91)</f>
         <v>28.333333333333329</v>
       </c>
+      <c r="J11" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="12" spans="2:10">
       <c r="B12" s="5"/>
@@ -2743,8 +2762,11 @@
         <v>15</v>
       </c>
       <c r="I12" s="4">
-        <f>SUM(E92:E104)</f>
-        <v>8.3333333333333321</v>
+        <f>SUM(E92:E108)</f>
+        <v>16.666666666666657</v>
+      </c>
+      <c r="J12" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="2:10">
@@ -2762,7 +2784,10 @@
       <c r="H13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I13" s="4"/>
+      <c r="I13" s="4">
+        <f>SUM(E109:E126)</f>
+        <v>12.500000000000004</v>
+      </c>
     </row>
     <row r="14" spans="2:10">
       <c r="C14" s="2">
@@ -2790,6 +2815,9 @@
       <c r="E15" s="4">
         <f t="shared" si="0"/>
         <v>1.0000000000000018</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="I15" s="4"/>
     </row>
@@ -2805,6 +2833,9 @@
         <f t="shared" si="0"/>
         <v>2.0000000000000009</v>
       </c>
+      <c r="H16" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="I16" s="4"/>
     </row>
     <row r="17" spans="2:9">
@@ -3932,74 +3963,255 @@
       </c>
     </row>
     <row r="98" spans="2:5">
-      <c r="C98" s="2"/>
-      <c r="D98" s="2"/>
-      <c r="E98" s="4"/>
+      <c r="B98" s="5">
+        <v>42935</v>
+      </c>
+      <c r="C98" s="2">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="D98" s="2">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="E98" s="4">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333215</v>
+      </c>
     </row>
     <row r="99" spans="2:5">
-      <c r="C99" s="2"/>
-      <c r="D99" s="2"/>
-      <c r="E99" s="4"/>
+      <c r="C99" s="2">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="D99" s="2">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="E99" s="4">
+        <f t="shared" si="0"/>
+        <v>1.4166666666666656</v>
+      </c>
     </row>
     <row r="100" spans="2:5">
       <c r="B100" s="5"/>
-      <c r="C100" s="2"/>
-      <c r="D100" s="2"/>
-      <c r="E100" s="4"/>
+      <c r="C100" s="2">
+        <v>0.52430555555555558</v>
+      </c>
+      <c r="D100" s="2">
+        <v>0.64236111111111105</v>
+      </c>
+      <c r="E100" s="4">
+        <f t="shared" si="0"/>
+        <v>2.8333333333333313</v>
+      </c>
     </row>
     <row r="101" spans="2:5">
-      <c r="C101" s="2"/>
-      <c r="D101" s="2"/>
-      <c r="E101" s="4"/>
+      <c r="B101" s="5">
+        <v>42937</v>
+      </c>
+      <c r="C101" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D101" s="2">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="E101" s="4">
+        <f t="shared" si="0"/>
+        <v>1.3333333333333339</v>
+      </c>
     </row>
     <row r="102" spans="2:5">
       <c r="B102" s="5"/>
-      <c r="C102" s="2"/>
-      <c r="D102" s="2"/>
-      <c r="E102" s="4"/>
+      <c r="C102" s="2">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="D102" s="2">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E102" s="4">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666607</v>
+      </c>
     </row>
     <row r="103" spans="2:5">
       <c r="B103" s="5"/>
-      <c r="C103" s="2"/>
-      <c r="D103" s="2"/>
-      <c r="E103" s="4"/>
+      <c r="C103" s="2">
+        <v>0.62152777777777779</v>
+      </c>
+      <c r="D103" s="2">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="E103" s="4">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333215</v>
+      </c>
     </row>
     <row r="104" spans="2:5">
       <c r="B104" s="5"/>
-      <c r="C104" s="2"/>
-      <c r="D104" s="2"/>
-      <c r="E104" s="4"/>
+      <c r="C104" s="2">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="D104" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E104" s="4">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333215</v>
+      </c>
     </row>
     <row r="105" spans="2:5">
-      <c r="C105" s="2"/>
-      <c r="D105" s="2"/>
-      <c r="E105" s="4"/>
+      <c r="C105" s="2">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="D105" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="E105" s="4">
+        <f t="shared" si="0"/>
+        <v>0.24999999999999911</v>
+      </c>
     </row>
     <row r="106" spans="2:5">
-      <c r="C106" s="2"/>
-      <c r="D106" s="2"/>
-      <c r="E106" s="4"/>
+      <c r="B106" s="5">
+        <v>42939</v>
+      </c>
+      <c r="C106" s="2">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D106" s="2">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="E106" s="4">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666607</v>
+      </c>
     </row>
     <row r="107" spans="2:5">
-      <c r="C107" s="2"/>
-      <c r="D107" s="2"/>
-      <c r="E107" s="4"/>
+      <c r="C107" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D107" s="2">
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="E107" s="4">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666696</v>
+      </c>
     </row>
     <row r="108" spans="2:5">
-      <c r="C108" s="2"/>
-      <c r="D108" s="2"/>
-      <c r="E108" s="4"/>
+      <c r="C108" s="2">
+        <v>0.84722222222222221</v>
+      </c>
+      <c r="D108" s="2">
+        <v>0.86805555555555547</v>
+      </c>
+      <c r="E108" s="4">
+        <f t="shared" si="0"/>
+        <v>0.49999999999999822</v>
+      </c>
     </row>
     <row r="109" spans="2:5">
-      <c r="C109" s="2"/>
-      <c r="D109" s="2"/>
-      <c r="E109" s="4"/>
+      <c r="B109" s="5">
+        <v>42940</v>
+      </c>
+      <c r="C109" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="D109" s="2">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="E109" s="4">
+        <f t="shared" si="0"/>
+        <v>1.8333333333333335</v>
+      </c>
     </row>
     <row r="110" spans="2:5">
       <c r="B110" s="5"/>
-      <c r="C110" s="2"/>
-      <c r="D110" s="2"/>
-      <c r="E110" s="4"/>
+      <c r="C110" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D110" s="2">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="E110" s="4">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333481</v>
+      </c>
+    </row>
+    <row r="111" spans="2:5">
+      <c r="C111" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D111" s="2">
+        <v>0.58680555555555558</v>
+      </c>
+      <c r="E111" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0833333333333348</v>
+      </c>
+    </row>
+    <row r="112" spans="2:5">
+      <c r="C112" s="2">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="D112" s="2">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="E112" s="4">
+        <f t="shared" si="0"/>
+        <v>2.0833333333333339</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5">
+      <c r="C113" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D113" s="2">
+        <v>0.78125</v>
+      </c>
+      <c r="E113" s="4">
+        <f t="shared" si="0"/>
+        <v>1.7499999999999991</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5">
+      <c r="B114" s="5">
+        <v>42941</v>
+      </c>
+      <c r="C114" s="2">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="D114" s="2">
+        <v>0.70486111111111116</v>
+      </c>
+      <c r="E114" s="4">
+        <f t="shared" si="0"/>
+        <v>3.2500000000000018</v>
+      </c>
+    </row>
+    <row r="115" spans="2:5">
+      <c r="C115" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D115" s="2">
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="E115" s="4">
+        <f t="shared" si="0"/>
+        <v>1.3333333333333313</v>
+      </c>
+    </row>
+    <row r="116" spans="2:5">
+      <c r="B116" s="5">
+        <v>42942</v>
+      </c>
+      <c r="C116" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D116" s="2">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="E116" s="4">
+        <f t="shared" si="0"/>
+        <v>0.83333333333333304</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>